<commit_message>
added english col names
</commit_message>
<xml_diff>
--- a/data/codebook.xlsx
+++ b/data/codebook.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Tejerina\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\H7Z10R6B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/RStudio WD/Projects/Computational Statistics/Homework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B66626-0AA1-3344-AF54-BA48D78E54DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7250"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="409">
   <si>
     <t>v2a1</t>
   </si>
@@ -876,13 +877,388 @@
   </si>
   <si>
     <t>Variable description</t>
+  </si>
+  <si>
+    <t>rent</t>
+  </si>
+  <si>
+    <t>room_overcrwd</t>
+  </si>
+  <si>
+    <t>bedroom_overcrwd</t>
+  </si>
+  <si>
+    <t>toilet</t>
+  </si>
+  <si>
+    <t>tablet</t>
+  </si>
+  <si>
+    <t>no_tablets</t>
+  </si>
+  <si>
+    <t>males</t>
+  </si>
+  <si>
+    <t>males_&lt;12</t>
+  </si>
+  <si>
+    <t>males_&gt;12</t>
+  </si>
+  <si>
+    <t>fem_&lt;12</t>
+  </si>
+  <si>
+    <t>fem_&gt;12</t>
+  </si>
+  <si>
+    <t>pers_&lt;12</t>
+  </si>
+  <si>
+    <t>pers_&gt;12</t>
+  </si>
+  <si>
+    <t>total_pers</t>
+  </si>
+  <si>
+    <t>total_fem</t>
+  </si>
+  <si>
+    <t>school_yrs</t>
+  </si>
+  <si>
+    <t>school_yrs_behind</t>
+  </si>
+  <si>
+    <t>English Variable Name</t>
+  </si>
+  <si>
+    <t>wall_brickblock</t>
+  </si>
+  <si>
+    <t>wall_socket</t>
+  </si>
+  <si>
+    <t>wall_prefcement</t>
+  </si>
+  <si>
+    <t>wall_waste</t>
+  </si>
+  <si>
+    <t>wall_wood</t>
+  </si>
+  <si>
+    <t>wall_zink</t>
+  </si>
+  <si>
+    <t>wall_fiber</t>
+  </si>
+  <si>
+    <t>wall_other</t>
+  </si>
+  <si>
+    <t>floor_cement</t>
+  </si>
+  <si>
+    <t>floor_other</t>
+  </si>
+  <si>
+    <t>floor_natural</t>
+  </si>
+  <si>
+    <t>floor_none</t>
+  </si>
+  <si>
+    <t>floor_wood</t>
+  </si>
+  <si>
+    <t>roof_zink</t>
+  </si>
+  <si>
+    <t>roof_fiber</t>
+  </si>
+  <si>
+    <t>roof_other</t>
+  </si>
+  <si>
+    <t>floor_mocerter</t>
+  </si>
+  <si>
+    <t>roof_cementmez</t>
+  </si>
+  <si>
+    <t>ceiling</t>
+  </si>
+  <si>
+    <t>water_inside</t>
+  </si>
+  <si>
+    <t>water_outside</t>
+  </si>
+  <si>
+    <t>water_none</t>
+  </si>
+  <si>
+    <t>elec_pub</t>
+  </si>
+  <si>
+    <t>elec_priv</t>
+  </si>
+  <si>
+    <t>elec_none</t>
+  </si>
+  <si>
+    <t>elec_coop</t>
+  </si>
+  <si>
+    <t>toilet_none</t>
+  </si>
+  <si>
+    <t>toilet_sewer</t>
+  </si>
+  <si>
+    <t>toilet_septic</t>
+  </si>
+  <si>
+    <t>toilet_let</t>
+  </si>
+  <si>
+    <t>toilet_other</t>
+  </si>
+  <si>
+    <t>cook_none</t>
+  </si>
+  <si>
+    <t>cook_elec</t>
+  </si>
+  <si>
+    <t>cook_gas</t>
+  </si>
+  <si>
+    <t>cook_char</t>
+  </si>
+  <si>
+    <t>rub_truck</t>
+  </si>
+  <si>
+    <t>rub_burn</t>
+  </si>
+  <si>
+    <t>rub_dig</t>
+  </si>
+  <si>
+    <t>rub_space</t>
+  </si>
+  <si>
+    <t>rub_water</t>
+  </si>
+  <si>
+    <t>rub_other</t>
+  </si>
+  <si>
+    <t>walls_bad</t>
+  </si>
+  <si>
+    <t>walls_regular</t>
+  </si>
+  <si>
+    <t>walls_good</t>
+  </si>
+  <si>
+    <t>roof_bad</t>
+  </si>
+  <si>
+    <t>roof_regular</t>
+  </si>
+  <si>
+    <t>roof_good</t>
+  </si>
+  <si>
+    <t>floor_bad</t>
+  </si>
+  <si>
+    <t>floor_regular</t>
+  </si>
+  <si>
+    <t>floor_good</t>
+  </si>
+  <si>
+    <t>disabled</t>
+  </si>
+  <si>
+    <t>&lt;10_yrs</t>
+  </si>
+  <si>
+    <t>married</t>
+  </si>
+  <si>
+    <t>couple</t>
+  </si>
+  <si>
+    <t>divorced</t>
+  </si>
+  <si>
+    <t>separated</t>
+  </si>
+  <si>
+    <t>widowed</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>spouse_partner</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>stepchild</t>
+  </si>
+  <si>
+    <t>inlaw_child</t>
+  </si>
+  <si>
+    <t>grandchild</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>inlaw_parent</t>
+  </si>
+  <si>
+    <t>sibling</t>
+  </si>
+  <si>
+    <t>inlaw_sibling</t>
+  </si>
+  <si>
+    <t>family_other</t>
+  </si>
+  <si>
+    <t>nonfamiliy</t>
+  </si>
+  <si>
+    <t>hh_children</t>
+  </si>
+  <si>
+    <t>hh_id</t>
+  </si>
+  <si>
+    <t>hh_adults</t>
+  </si>
+  <si>
+    <t>hh_senior</t>
+  </si>
+  <si>
+    <t>hh_total</t>
+  </si>
+  <si>
+    <t>ed_head_m</t>
+  </si>
+  <si>
+    <t>ed_head_f</t>
+  </si>
+  <si>
+    <t>ed_level1</t>
+  </si>
+  <si>
+    <t>ed_level2</t>
+  </si>
+  <si>
+    <t>ed_level3</t>
+  </si>
+  <si>
+    <t>ed_level4</t>
+  </si>
+  <si>
+    <t>ed_level5</t>
+  </si>
+  <si>
+    <t>ed_level6</t>
+  </si>
+  <si>
+    <t>ed_level7</t>
+  </si>
+  <si>
+    <t>ed_level8</t>
+  </si>
+  <si>
+    <t>ed_level9</t>
+  </si>
+  <si>
+    <t>owner_full</t>
+  </si>
+  <si>
+    <t>owner_paying</t>
+  </si>
+  <si>
+    <t>owner_rent</t>
+  </si>
+  <si>
+    <t>owner_precarious</t>
+  </si>
+  <si>
+    <t>owner_other</t>
+  </si>
+  <si>
+    <t>no_mobilephone</t>
+  </si>
+  <si>
+    <t>region1</t>
+  </si>
+  <si>
+    <t>region2</t>
+  </si>
+  <si>
+    <t>region3</t>
+  </si>
+  <si>
+    <t>region4</t>
+  </si>
+  <si>
+    <t>region5</t>
+  </si>
+  <si>
+    <t>region6</t>
+  </si>
+  <si>
+    <t>age_sqr</t>
+  </si>
+  <si>
+    <t>hh_total_sqr</t>
+  </si>
+  <si>
+    <t>school_yrs_sqr</t>
+  </si>
+  <si>
+    <t>ed_head_m_sqr</t>
+  </si>
+  <si>
+    <t>hh_children_sqr</t>
+  </si>
+  <si>
+    <t>overcrowding_sqr</t>
+  </si>
+  <si>
+    <t>dependency_sqr</t>
+  </si>
+  <si>
+    <t>meaneduc_sqr</t>
+  </si>
+  <si>
+    <t>Age_sqr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -894,6 +1270,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -919,12 +1301,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -940,7 +1327,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1235,1155 +1622,1584 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B142"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143:XFD143"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="62.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="4" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="4" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="4" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="4" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="4" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="4" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C54" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="4" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="4" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="4" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C58" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="4" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="4" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="4" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="4" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C62" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="4" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C63" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C64" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="4" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="4" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="4" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C67" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="4" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C68" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="4" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="4" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C70" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="4" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C71" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="4" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C72" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="4" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C73" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="4" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="4" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C76" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="4" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C77" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="4" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C78" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="4" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C79" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C80" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="4" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C81" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C82" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="4" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C83" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="4" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C84" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="4" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C85" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="4" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C86" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="4" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C87" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="4" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C88" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="4" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C89" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="4" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C90" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C91" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C92" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="4" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C93" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C94" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C95" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>94</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="4" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C96" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C97" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C98" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="4" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C99" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="4" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C100" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="4" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C101" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="4" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C102" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="4" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C103" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="4" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C104" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="4" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C105" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C106" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C107" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C108" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C109" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C110" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C111" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="4" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C112" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>111</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="4" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C113" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>112</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C114" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>113</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="4" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C115" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C116" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>115</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="4" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C117" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>116</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="4" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C118" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>117</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="4" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C119" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>118</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="4" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C120" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>119</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="4" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C121" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>120</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="4" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C122" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>121</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="4" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C123" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>122</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="4" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C124" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>123</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="4" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C125" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>124</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="4" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C126" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>125</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="4" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C127" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>126</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C128" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="4" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C129" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="4" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C130" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="4" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C131" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="4" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C132" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="4" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C133" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="4" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C134" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="4" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C135" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="4" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C136" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="4" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C137" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="4" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C138" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C139" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>138</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="4" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C140" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>139</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="4" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C141" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>140</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="4" t="s">
         <v>281</v>
       </c>
+      <c r="C142" t="s">
+        <v>408</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added additional names to codebook
</commit_message>
<xml_diff>
--- a/data/codebook.xlsx
+++ b/data/codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/RStudio WD/Projects/Computational Statistics/Homework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B66626-0AA1-3344-AF54-BA48D78E54DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3B104B-089A-F74E-989C-F8253DC39F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="414">
   <si>
     <t>v2a1</t>
   </si>
@@ -1252,6 +1252,21 @@
   </si>
   <si>
     <t>Age_sqr</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>a unique identifier for each row</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>the target is an ordinal variable indicating groups of income levels</t>
   </si>
 </sst>
 </file>
@@ -1623,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C142"/>
+  <dimension ref="A1:C144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1649,1553 +1664,1575 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>412</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>141</v>
+        <v>411</v>
       </c>
       <c r="C2" t="s">
-        <v>284</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" t="s">
-        <v>285</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
-        <v>288</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>297</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s">
-        <v>299</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s">
-        <v>302</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C32" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C33" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C37" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C39" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C40" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C41" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C42" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C43" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C44" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C45" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C47" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C50" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C51" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C52" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C53" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C54" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C55" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C56" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C59" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C60" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C61" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C62" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C63" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C64" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C65" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C66" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C67" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C68" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C69" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C70" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C71" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C72" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C73" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C74" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C75" t="s">
-        <v>73</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C77" t="s">
-        <v>353</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C78" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C79" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C80" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C81" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C82" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C83" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C84" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C85" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C86" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C87" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C88" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C89" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C90" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C91" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C92" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C93" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C94" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C95" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C96" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C97" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C98" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C100" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C101" t="s">
-        <v>99</v>
+        <v>376</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C102" t="s">
-        <v>377</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C103" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C104" t="s">
-        <v>102</v>
+        <v>378</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C105" t="s">
-        <v>379</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C106" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C107" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C108" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C109" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C110" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C111" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C112" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C113" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C114" t="s">
-        <v>112</v>
+        <v>387</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C115" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C116" t="s">
-        <v>388</v>
+        <v>113</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C117" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C118" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C119" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C120" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C121" t="s">
-        <v>119</v>
+        <v>392</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C123" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C124" t="s">
-        <v>393</v>
+        <v>121</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C125" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C126" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C127" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C128" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C129" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C130" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C131" t="s">
-        <v>129</v>
+        <v>399</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C132" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C134" t="s">
-        <v>402</v>
+        <v>131</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C135" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C136" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C137" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C138" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C139" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C140" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C141" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>139</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C142" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>140</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C143" t="s">
         <v>408</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>409</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C144" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed some variable names
</commit_message>
<xml_diff>
--- a/data/codebook.xlsx
+++ b/data/codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/RStudio WD/Projects/Computational Statistics/Homework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3B104B-089A-F74E-989C-F8253DC39F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7273B6EA-0A6A-9A45-AE47-D18189FE21AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -900,24 +900,6 @@
     <t>males</t>
   </si>
   <si>
-    <t>males_&lt;12</t>
-  </si>
-  <si>
-    <t>males_&gt;12</t>
-  </si>
-  <si>
-    <t>fem_&lt;12</t>
-  </si>
-  <si>
-    <t>fem_&gt;12</t>
-  </si>
-  <si>
-    <t>pers_&lt;12</t>
-  </si>
-  <si>
-    <t>pers_&gt;12</t>
-  </si>
-  <si>
     <t>total_pers</t>
   </si>
   <si>
@@ -1086,9 +1068,6 @@
     <t>disabled</t>
   </si>
   <si>
-    <t>&lt;10_yrs</t>
-  </si>
-  <si>
     <t>married</t>
   </si>
   <si>
@@ -1267,6 +1246,27 @@
   </si>
   <si>
     <t>the target is an ordinal variable indicating groups of income levels</t>
+  </si>
+  <si>
+    <t>males_under12</t>
+  </si>
+  <si>
+    <t>males_over12</t>
+  </si>
+  <si>
+    <t>fem_under12</t>
+  </si>
+  <si>
+    <t>fem_over12</t>
+  </si>
+  <si>
+    <t>pers_under12</t>
+  </si>
+  <si>
+    <t>pers_over12</t>
+  </si>
+  <si>
+    <t>under10_yrs</t>
   </si>
 </sst>
 </file>
@@ -1640,8 +1640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="B148" sqref="B148"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1659,18 +1659,18 @@
         <v>283</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="C2" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1769,7 +1769,7 @@
         <v>149</v>
       </c>
       <c r="C11" t="s">
-        <v>291</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1780,7 +1780,7 @@
         <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>292</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1802,7 +1802,7 @@
         <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>293</v>
+        <v>409</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1813,7 +1813,7 @@
         <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>294</v>
+        <v>410</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1824,7 +1824,7 @@
         <v>154</v>
       </c>
       <c r="C16" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1835,7 +1835,7 @@
         <v>155</v>
       </c>
       <c r="C17" t="s">
-        <v>295</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1846,7 +1846,7 @@
         <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>296</v>
+        <v>412</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1857,7 +1857,7 @@
         <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1890,7 +1890,7 @@
         <v>160</v>
       </c>
       <c r="C22" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1901,7 +1901,7 @@
         <v>161</v>
       </c>
       <c r="C23" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1923,7 +1923,7 @@
         <v>163</v>
       </c>
       <c r="C25" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1934,7 +1934,7 @@
         <v>164</v>
       </c>
       <c r="C26" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1945,7 +1945,7 @@
         <v>165</v>
       </c>
       <c r="C27" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1956,7 +1956,7 @@
         <v>166</v>
       </c>
       <c r="C28" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1967,7 +1967,7 @@
         <v>167</v>
       </c>
       <c r="C29" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1978,7 +1978,7 @@
         <v>168</v>
       </c>
       <c r="C30" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1989,7 +1989,7 @@
         <v>169</v>
       </c>
       <c r="C31" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2000,7 +2000,7 @@
         <v>170</v>
       </c>
       <c r="C32" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2011,7 +2011,7 @@
         <v>171</v>
       </c>
       <c r="C33" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2022,7 +2022,7 @@
         <v>172</v>
       </c>
       <c r="C34" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2033,7 +2033,7 @@
         <v>173</v>
       </c>
       <c r="C35" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2044,7 +2044,7 @@
         <v>174</v>
       </c>
       <c r="C36" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2055,7 +2055,7 @@
         <v>175</v>
       </c>
       <c r="C37" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2066,7 +2066,7 @@
         <v>176</v>
       </c>
       <c r="C38" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2077,7 +2077,7 @@
         <v>177</v>
       </c>
       <c r="C39" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2088,7 +2088,7 @@
         <v>178</v>
       </c>
       <c r="C40" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2099,7 +2099,7 @@
         <v>179</v>
       </c>
       <c r="C41" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2110,7 +2110,7 @@
         <v>180</v>
       </c>
       <c r="C42" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2121,7 +2121,7 @@
         <v>181</v>
       </c>
       <c r="C43" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2132,7 +2132,7 @@
         <v>182</v>
       </c>
       <c r="C44" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2143,7 +2143,7 @@
         <v>183</v>
       </c>
       <c r="C45" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2154,7 +2154,7 @@
         <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2165,7 +2165,7 @@
         <v>185</v>
       </c>
       <c r="C47" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2176,7 +2176,7 @@
         <v>186</v>
       </c>
       <c r="C48" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2187,7 +2187,7 @@
         <v>187</v>
       </c>
       <c r="C49" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2198,7 +2198,7 @@
         <v>188</v>
       </c>
       <c r="C50" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2209,7 +2209,7 @@
         <v>189</v>
       </c>
       <c r="C51" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2220,7 +2220,7 @@
         <v>190</v>
       </c>
       <c r="C52" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2231,7 +2231,7 @@
         <v>191</v>
       </c>
       <c r="C53" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2242,7 +2242,7 @@
         <v>192</v>
       </c>
       <c r="C54" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2253,7 +2253,7 @@
         <v>193</v>
       </c>
       <c r="C55" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2264,7 +2264,7 @@
         <v>194</v>
       </c>
       <c r="C56" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2275,7 +2275,7 @@
         <v>195</v>
       </c>
       <c r="C57" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2286,7 +2286,7 @@
         <v>196</v>
       </c>
       <c r="C58" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2297,7 +2297,7 @@
         <v>197</v>
       </c>
       <c r="C59" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2308,7 +2308,7 @@
         <v>198</v>
       </c>
       <c r="C60" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2319,7 +2319,7 @@
         <v>199</v>
       </c>
       <c r="C61" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2330,7 +2330,7 @@
         <v>200</v>
       </c>
       <c r="C62" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2341,7 +2341,7 @@
         <v>201</v>
       </c>
       <c r="C63" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2352,7 +2352,7 @@
         <v>202</v>
       </c>
       <c r="C64" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2363,7 +2363,7 @@
         <v>203</v>
       </c>
       <c r="C65" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2374,7 +2374,7 @@
         <v>204</v>
       </c>
       <c r="C66" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2385,7 +2385,7 @@
         <v>205</v>
       </c>
       <c r="C67" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2396,7 +2396,7 @@
         <v>206</v>
       </c>
       <c r="C68" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2407,7 +2407,7 @@
         <v>207</v>
       </c>
       <c r="C69" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2418,7 +2418,7 @@
         <v>208</v>
       </c>
       <c r="C70" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2429,7 +2429,7 @@
         <v>209</v>
       </c>
       <c r="C71" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2440,7 +2440,7 @@
         <v>210</v>
       </c>
       <c r="C72" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2451,7 +2451,7 @@
         <v>211</v>
       </c>
       <c r="C73" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2462,7 +2462,7 @@
         <v>212</v>
       </c>
       <c r="C74" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2473,7 +2473,7 @@
         <v>213</v>
       </c>
       <c r="C75" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2506,7 +2506,7 @@
         <v>216</v>
       </c>
       <c r="C78" t="s">
-        <v>353</v>
+        <v>413</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2517,7 +2517,7 @@
         <v>217</v>
       </c>
       <c r="C79" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2528,7 +2528,7 @@
         <v>218</v>
       </c>
       <c r="C80" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2539,7 +2539,7 @@
         <v>219</v>
       </c>
       <c r="C81" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2550,7 +2550,7 @@
         <v>220</v>
       </c>
       <c r="C82" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2561,7 +2561,7 @@
         <v>221</v>
       </c>
       <c r="C83" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2572,7 +2572,7 @@
         <v>222</v>
       </c>
       <c r="C84" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2583,7 +2583,7 @@
         <v>223</v>
       </c>
       <c r="C85" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2594,7 +2594,7 @@
         <v>224</v>
       </c>
       <c r="C86" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2605,7 +2605,7 @@
         <v>225</v>
       </c>
       <c r="C87" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2616,7 +2616,7 @@
         <v>226</v>
       </c>
       <c r="C88" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2627,7 +2627,7 @@
         <v>227</v>
       </c>
       <c r="C89" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2638,7 +2638,7 @@
         <v>228</v>
       </c>
       <c r="C90" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2649,7 +2649,7 @@
         <v>229</v>
       </c>
       <c r="C91" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2660,7 +2660,7 @@
         <v>230</v>
       </c>
       <c r="C92" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2671,7 +2671,7 @@
         <v>231</v>
       </c>
       <c r="C93" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2682,7 +2682,7 @@
         <v>232</v>
       </c>
       <c r="C94" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2693,7 +2693,7 @@
         <v>233</v>
       </c>
       <c r="C95" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2704,7 +2704,7 @@
         <v>234</v>
       </c>
       <c r="C96" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2715,7 +2715,7 @@
         <v>235</v>
       </c>
       <c r="C97" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2726,7 +2726,7 @@
         <v>236</v>
       </c>
       <c r="C98" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -2737,7 +2737,7 @@
         <v>237</v>
       </c>
       <c r="C99" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2748,7 +2748,7 @@
         <v>238</v>
       </c>
       <c r="C100" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2759,7 +2759,7 @@
         <v>239</v>
       </c>
       <c r="C101" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -2781,7 +2781,7 @@
         <v>241</v>
       </c>
       <c r="C103" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -2792,7 +2792,7 @@
         <v>242</v>
       </c>
       <c r="C104" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -2814,7 +2814,7 @@
         <v>244</v>
       </c>
       <c r="C106" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -2825,7 +2825,7 @@
         <v>245</v>
       </c>
       <c r="C107" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -2836,7 +2836,7 @@
         <v>246</v>
       </c>
       <c r="C108" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -2847,7 +2847,7 @@
         <v>247</v>
       </c>
       <c r="C109" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -2858,7 +2858,7 @@
         <v>248</v>
       </c>
       <c r="C110" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -2869,7 +2869,7 @@
         <v>249</v>
       </c>
       <c r="C111" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -2880,7 +2880,7 @@
         <v>250</v>
       </c>
       <c r="C112" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -2891,7 +2891,7 @@
         <v>251</v>
       </c>
       <c r="C113" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -2902,7 +2902,7 @@
         <v>252</v>
       </c>
       <c r="C114" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -2935,7 +2935,7 @@
         <v>255</v>
       </c>
       <c r="C117" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -2946,7 +2946,7 @@
         <v>256</v>
       </c>
       <c r="C118" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -2957,7 +2957,7 @@
         <v>257</v>
       </c>
       <c r="C119" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -2968,7 +2968,7 @@
         <v>258</v>
       </c>
       <c r="C120" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -2979,7 +2979,7 @@
         <v>259</v>
       </c>
       <c r="C121" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -3023,7 +3023,7 @@
         <v>263</v>
       </c>
       <c r="C125" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -3034,7 +3034,7 @@
         <v>264</v>
       </c>
       <c r="C126" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -3045,7 +3045,7 @@
         <v>265</v>
       </c>
       <c r="C127" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -3056,7 +3056,7 @@
         <v>266</v>
       </c>
       <c r="C128" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -3067,7 +3067,7 @@
         <v>267</v>
       </c>
       <c r="C129" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -3078,7 +3078,7 @@
         <v>268</v>
       </c>
       <c r="C130" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -3089,7 +3089,7 @@
         <v>269</v>
       </c>
       <c r="C131" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -3133,7 +3133,7 @@
         <v>273</v>
       </c>
       <c r="C135" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -3144,7 +3144,7 @@
         <v>274</v>
       </c>
       <c r="C136" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -3155,7 +3155,7 @@
         <v>275</v>
       </c>
       <c r="C137" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -3166,7 +3166,7 @@
         <v>276</v>
       </c>
       <c r="C138" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -3177,7 +3177,7 @@
         <v>277</v>
       </c>
       <c r="C139" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -3188,7 +3188,7 @@
         <v>278</v>
       </c>
       <c r="C140" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -3199,7 +3199,7 @@
         <v>279</v>
       </c>
       <c r="C141" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -3210,7 +3210,7 @@
         <v>280</v>
       </c>
       <c r="C142" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -3221,18 +3221,18 @@
         <v>281</v>
       </c>
       <c r="C143" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C144" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>